<commit_message>
Data loading - Weather, Course, Postcodes
Long/lat postcode updates, updated weather data, updates to unit list based on data from CAM office.
</commit_message>
<xml_diff>
--- a/data/accomodation_data/Halls_Details.xlsx
+++ b/data/accomodation_data/Halls_Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry\Documents\University\Year 3\Dissertation\data\accomodation_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry\Documents\University\Year 3\Dissertation\UoP_Dissertation\data\accomodation_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{166A6C06-8BE7-4666-9C9F-369B08ADDC1C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FAA750-61D7-4DD5-B219-32E4551B4090}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18210" xr2:uid="{8B5462B4-FDFA-4E96-AB7F-7791521926D9}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Floors</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>Chaucer House</t>
   </si>
@@ -58,22 +52,92 @@
   </si>
   <si>
     <t>Margaret Rule Hall</t>
+  </si>
+  <si>
+    <t>building_name</t>
+  </si>
+  <si>
+    <t>street_address1</t>
+  </si>
+  <si>
+    <t>street_address2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>Portsmouth</t>
+  </si>
+  <si>
+    <t>Hampshire</t>
+  </si>
+  <si>
+    <t>Stanhope Rd</t>
+  </si>
+  <si>
+    <t>PO11DZ</t>
+  </si>
+  <si>
+    <t>PO12DR</t>
+  </si>
+  <si>
+    <t>Greetham St</t>
+  </si>
+  <si>
+    <t>PO54FB</t>
+  </si>
+  <si>
+    <t>PO12DS</t>
+  </si>
+  <si>
+    <t>Isambard Brunel Road</t>
+  </si>
+  <si>
+    <t>32 Isambard Brunel Road</t>
+  </si>
+  <si>
+    <t>PO12SP</t>
+  </si>
+  <si>
+    <t>28 Guildhall Walk</t>
+  </si>
+  <si>
+    <t>PO12DD</t>
+  </si>
+  <si>
+    <t>Middle Street</t>
+  </si>
+  <si>
+    <t>Southsea</t>
+  </si>
+  <si>
+    <t>PO54AY</t>
+  </si>
+  <si>
+    <t>The Mary Rose Street</t>
+  </si>
+  <si>
+    <t>PO12BL</t>
+  </si>
+  <si>
+    <t>Southsea Terrace</t>
+  </si>
+  <si>
+    <t>PO53AP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -103,7 +167,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,68 +482,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4404756-0FD8-4AFB-98E5-FC996419F089}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>